<commit_message>
Add second office hw
</commit_message>
<xml_diff>
--- a/3 term/homeworks/6. Office modules/23_16/test_data/tender.xlsx
+++ b/3 term/homeworks/6. Office modules/23_16/test_data/tender.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,28 @@
       <c r="D3" t="inlineStr">
         <is>
           <t>condor@com.ua</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>S03</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>max@com.ua</t>
         </is>
       </c>
     </row>
@@ -500,7 +522,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,6 +563,18 @@
       <c r="B3" t="inlineStr">
         <is>
           <t>Ручка кулькова</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>P03</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Папір</t>
         </is>
       </c>
     </row>
@@ -555,7 +589,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,6 +663,50 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>S02</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>P01</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2,6</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>S03</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>P01</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3,0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>